<commit_message>
feat(pipelining): add MOVS testing program #18
</commit_message>
<xml_diff>
--- a/programs/pipelining/pipeliningdataprocessingregisterinstructionsnohazards.xlsx
+++ b/programs/pipelining/pipeliningdataprocessingregisterinstructionsnohazards.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vacla\Projects\cpu\programs\pipelining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF8375DA-5765-4AC0-827F-2C7551538316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A63AF0AE-6F9C-45D2-B69E-FDD7CA981CEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E410B2C1-F054-41C4-A96D-F1120FBD95E0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Code" sheetId="1" r:id="rId1"/>
+    <sheet name="Pipeline" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="49">
   <si>
     <t>Hex</t>
   </si>
@@ -172,6 +173,15 @@
   </si>
   <si>
     <t>0x3000</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>E1</t>
+  </si>
+  <si>
+    <t>E2</t>
   </si>
 </sst>
 </file>
@@ -555,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E17FB6-AC76-4C3E-BEFA-6AB3607784FD}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="A8:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1258,6 +1268,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="M4:P4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:R5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="K6:P6"/>
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="K2:M2"/>
@@ -1267,19 +1287,129 @@
     <mergeCell ref="K3:N3"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="K6:P6"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="M4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:R5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48E91437-0323-4525-AFEC-B50198BB676A}">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" t="s">
+        <v>47</v>
+      </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>